<commit_message>
hightlight with function interface and main frame integration completed
</commit_message>
<xml_diff>
--- a/Source/MetroSystem/data/edges_SZ.xlsx
+++ b/Source/MetroSystem/data/edges_SZ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\城大\课程\Year 3 Sem A\CS3343\CS3343_Group6\MetroSystem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lww887\3343\CS3343_Group6\Source\MetroSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA3A53B-7AD6-441A-A732-AC36A819394F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15792" yWindow="3804" windowWidth="11052" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15795" yWindow="3810" windowWidth="11055" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,104 +26,41 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>start_station</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>ssds</t>
   </si>
   <si>
-    <t>end_station</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>sdsd</t>
   </si>
   <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>sdsds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00F6BB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9C856C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,21 +75,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,16 +363,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C274"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D270" sqref="D270"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,3007 +383,3015 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>5</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>7</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>8</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>9</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10">
         <v>10</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>11</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>12</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>13</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:3">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>14</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15">
         <v>15</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:3">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16">
         <v>16</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:3">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>17</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18">
         <v>18</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19">
         <v>19</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:3">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20">
         <v>20</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+    <row r="21" spans="1:3">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21">
         <v>21</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+    <row r="22" spans="1:3">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>22</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    <row r="23" spans="1:3">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23">
         <v>23</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="24" spans="1:3">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24">
         <v>24</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+    <row r="25" spans="1:3">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25">
         <v>25</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+    <row r="26" spans="1:3">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26">
         <v>26</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:3">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27">
         <v>27</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+    <row r="28" spans="1:3">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28">
         <v>28</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+    <row r="29" spans="1:3">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29">
         <v>29</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+    <row r="30" spans="1:3">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30">
         <v>30</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+    <row r="31" spans="1:3">
+      <c r="A31">
         <v>31</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31">
         <v>32</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+    <row r="32" spans="1:3">
+      <c r="A32">
         <v>32</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32">
         <v>33</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+    <row r="33" spans="1:3">
+      <c r="A33">
         <v>33</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33">
         <v>34</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+    <row r="34" spans="1:3">
+      <c r="A34">
         <v>34</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34">
         <v>35</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+    <row r="35" spans="1:3">
+      <c r="A35">
         <v>35</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35">
         <v>36</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+    <row r="36" spans="1:3">
+      <c r="A36">
         <v>36</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36">
         <v>37</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+    <row r="37" spans="1:3">
+      <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37">
         <v>38</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+    <row r="38" spans="1:3">
+      <c r="A38">
         <v>38</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38">
         <v>39</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+    <row r="39" spans="1:3">
+      <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39">
         <v>40</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+    <row r="40" spans="1:3">
+      <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40">
         <v>41</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+    <row r="41" spans="1:3">
+      <c r="A41">
         <v>41</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41">
         <v>15</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+    <row r="42" spans="1:3">
+      <c r="A42">
         <v>15</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42">
         <v>42</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
+    <row r="43" spans="1:3">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43">
         <v>43</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
+    <row r="44" spans="1:3">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44">
         <v>44</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+    <row r="45" spans="1:3">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45">
         <v>45</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+    <row r="46" spans="1:3">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46">
         <v>46</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
+    <row r="47" spans="1:3">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47">
         <v>47</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
+    <row r="48" spans="1:3">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48">
         <v>48</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
+    <row r="49" spans="1:3">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49">
         <v>49</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6">
+    <row r="50" spans="1:3">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50">
         <v>50</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
+    <row r="51" spans="1:3">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51">
         <v>90</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6">
+    <row r="52" spans="1:3">
+      <c r="A52">
         <v>90</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52">
         <v>51</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+    <row r="53" spans="1:3">
+      <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53">
         <v>52</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
+    <row r="54" spans="1:3">
+      <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54">
         <v>53</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
+    <row r="55" spans="1:3">
+      <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55">
         <v>4</v>
       </c>
       <c r="C55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6">
+    <row r="56" spans="1:3">
+      <c r="A56">
         <v>4</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56">
         <v>54</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+    <row r="57" spans="1:3">
+      <c r="A57">
         <v>54</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57">
         <v>55</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
+    <row r="58" spans="1:3">
+      <c r="A58">
         <v>55</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58">
         <v>56</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
+    <row r="59" spans="1:3">
+      <c r="A59">
         <v>56</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59">
         <v>57</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6">
+    <row r="60" spans="1:3">
+      <c r="A60">
         <v>57</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60">
         <v>58</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6">
+    <row r="61" spans="1:3">
+      <c r="A61">
         <v>58</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61">
         <v>59</v>
       </c>
       <c r="C61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6">
+    <row r="62" spans="1:3">
+      <c r="A62">
         <v>59</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62">
         <v>176</v>
       </c>
       <c r="C62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
+    <row r="63" spans="1:3">
+      <c r="A63">
         <v>176</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63">
         <v>177</v>
       </c>
       <c r="C63">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6">
+    <row r="64" spans="1:3">
+      <c r="A64">
         <v>177</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64">
         <v>178</v>
       </c>
       <c r="C64">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6">
+    <row r="65" spans="1:3">
+      <c r="A65">
         <v>178</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65">
         <v>179</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="6">
+    <row r="66" spans="1:3">
+      <c r="A66">
         <v>179</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66">
         <v>180</v>
       </c>
       <c r="C66">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
+    <row r="67" spans="1:3">
+      <c r="A67">
         <v>180</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67">
         <v>181</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="7">
+    <row r="68" spans="1:3">
+      <c r="A68">
         <v>60</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68">
         <v>61</v>
       </c>
       <c r="C68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="7">
+    <row r="69" spans="1:3">
+      <c r="A69">
         <v>61</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69">
         <v>62</v>
       </c>
       <c r="C69">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="7">
+    <row r="70" spans="1:3">
+      <c r="A70">
         <v>62</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70">
         <v>9</v>
       </c>
       <c r="C70">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="7">
+    <row r="71" spans="1:3">
+      <c r="A71">
         <v>9</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71">
         <v>50</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="7">
+    <row r="72" spans="1:3">
+      <c r="A72">
         <v>50</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72">
         <v>63</v>
       </c>
       <c r="C72">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="7">
+    <row r="73" spans="1:3">
+      <c r="A73">
         <v>63</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73">
         <v>64</v>
       </c>
       <c r="C73">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="7">
+    <row r="74" spans="1:3">
+      <c r="A74">
         <v>64</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74">
         <v>65</v>
       </c>
       <c r="C74">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7">
+    <row r="75" spans="1:3">
+      <c r="A75">
         <v>65</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75">
         <v>66</v>
       </c>
       <c r="C75">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="7">
+    <row r="76" spans="1:3">
+      <c r="A76">
         <v>66</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76">
         <v>67</v>
       </c>
       <c r="C76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7">
+    <row r="77" spans="1:3">
+      <c r="A77">
         <v>67</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77">
         <v>3</v>
       </c>
       <c r="C77">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7">
-        <v>3</v>
-      </c>
-      <c r="B78" s="7">
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78">
         <v>68</v>
       </c>
       <c r="C78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7">
+    <row r="79" spans="1:3">
+      <c r="A79">
         <v>68</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79">
         <v>69</v>
       </c>
       <c r="C79">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="7">
+    <row r="80" spans="1:3">
+      <c r="A80">
         <v>69</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B80">
         <v>70</v>
       </c>
       <c r="C80">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="7">
+    <row r="81" spans="1:3">
+      <c r="A81">
         <v>70</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81">
         <v>71</v>
       </c>
       <c r="C81">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="7">
+    <row r="82" spans="1:3">
+      <c r="A82">
         <v>71</v>
       </c>
-      <c r="B82" s="7">
+      <c r="B82">
         <v>72</v>
       </c>
       <c r="C82">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="7">
+    <row r="83" spans="1:3">
+      <c r="A83">
         <v>72</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83">
         <v>73</v>
       </c>
       <c r="C83">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
+    <row r="84" spans="1:3">
+      <c r="A84">
         <v>73</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84">
         <v>74</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="7">
+    <row r="85" spans="1:3">
+      <c r="A85">
         <v>74</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85">
         <v>75</v>
       </c>
       <c r="C85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="7">
+    <row r="86" spans="1:3">
+      <c r="A86">
         <v>75</v>
       </c>
-      <c r="B86" s="7">
+      <c r="B86">
         <v>76</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="7">
+    <row r="87" spans="1:3">
+      <c r="A87">
         <v>76</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87">
         <v>77</v>
       </c>
       <c r="C87">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="7">
+    <row r="88" spans="1:3">
+      <c r="A88">
         <v>77</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B88">
         <v>78</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="7">
+    <row r="89" spans="1:3">
+      <c r="A89">
         <v>78</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89">
         <v>79</v>
       </c>
       <c r="C89">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7">
+    <row r="90" spans="1:3">
+      <c r="A90">
         <v>79</v>
       </c>
-      <c r="B90" s="7">
+      <c r="B90">
         <v>80</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7">
+    <row r="91" spans="1:3">
+      <c r="A91">
         <v>80</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91">
         <v>81</v>
       </c>
       <c r="C91">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="7">
+    <row r="92" spans="1:3">
+      <c r="A92">
         <v>81</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92">
         <v>82</v>
       </c>
       <c r="C92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="7">
+    <row r="93" spans="1:3">
+      <c r="A93">
         <v>82</v>
       </c>
-      <c r="B93" s="7">
+      <c r="B93">
         <v>83</v>
       </c>
       <c r="C93">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7">
+    <row r="94" spans="1:3">
+      <c r="A94">
         <v>83</v>
       </c>
-      <c r="B94" s="7">
+      <c r="B94">
         <v>84</v>
       </c>
       <c r="C94">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="7">
+    <row r="95" spans="1:3">
+      <c r="A95">
         <v>84</v>
       </c>
-      <c r="B95" s="7">
+      <c r="B95">
         <v>85</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="7">
+    <row r="96" spans="1:3">
+      <c r="A96">
         <v>85</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96">
         <v>86</v>
       </c>
       <c r="C96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
+    <row r="97" spans="1:3">
+      <c r="A97">
         <v>86</v>
       </c>
-      <c r="B97" s="7">
+      <c r="B97">
         <v>87</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="98" spans="1:3">
+      <c r="A98">
         <v>88</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
         <v>89</v>
       </c>
       <c r="C98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+    <row r="99" spans="1:3">
+      <c r="A99">
         <v>89</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
         <v>8</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+    <row r="100" spans="1:3">
+      <c r="A100">
         <v>8</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
         <v>90</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101" spans="1:3">
+      <c r="A101">
         <v>90</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101">
         <v>63</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+    <row r="102" spans="1:3">
+      <c r="A102">
         <v>63</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102">
         <v>91</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103" spans="1:3">
+      <c r="A103">
         <v>91</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103">
         <v>92</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104" spans="1:3">
+      <c r="A104">
         <v>92</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
         <v>93</v>
       </c>
       <c r="C104">
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+    <row r="105" spans="1:3">
+      <c r="A105">
         <v>93</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
         <v>94</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+    <row r="106" spans="1:3">
+      <c r="A106">
         <v>94</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106">
         <v>95</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+    <row r="107" spans="1:3">
+      <c r="A107">
         <v>95</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107">
         <v>96</v>
       </c>
       <c r="C107">
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108" spans="1:3">
+      <c r="A108">
         <v>96</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108">
         <v>97</v>
       </c>
       <c r="C108">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+    <row r="109" spans="1:3">
+      <c r="A109">
         <v>97</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109">
         <v>98</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+    <row r="110" spans="1:3">
+      <c r="A110">
         <v>98</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110">
         <v>99</v>
       </c>
       <c r="C110">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+    <row r="111" spans="1:3">
+      <c r="A111">
         <v>99</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111">
         <v>100</v>
       </c>
       <c r="C111">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+    <row r="112" spans="1:3">
+      <c r="A112">
         <v>100</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112">
         <v>101</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+    <row r="113" spans="1:3">
+      <c r="A113">
         <v>101</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113">
         <v>102</v>
       </c>
       <c r="C113">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+    <row r="114" spans="1:3">
+      <c r="A114">
         <v>102</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114">
         <v>103</v>
       </c>
       <c r="C114">
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+    <row r="115" spans="1:3">
+      <c r="A115">
         <v>103</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>104</v>
       </c>
       <c r="C115">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+    <row r="116" spans="1:3">
+      <c r="A116">
         <v>104</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116">
         <v>105</v>
       </c>
       <c r="C116">
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+    <row r="117" spans="1:3">
+      <c r="A117">
         <v>105</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117">
         <v>106</v>
       </c>
       <c r="C117">
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+    <row r="118" spans="1:3">
+      <c r="A118">
         <v>106</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118">
         <v>107</v>
       </c>
       <c r="C118">
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+    <row r="119" spans="1:3">
+      <c r="A119">
         <v>107</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119">
         <v>108</v>
       </c>
       <c r="C119">
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+    <row r="120" spans="1:3">
+      <c r="A120">
         <v>31</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120">
         <v>109</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+    <row r="121" spans="1:3">
+      <c r="A121">
         <v>109</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121">
         <v>110</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+    <row r="122" spans="1:3">
+      <c r="A122">
         <v>110</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122">
         <v>111</v>
       </c>
       <c r="C122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+    <row r="123" spans="1:3">
+      <c r="A123">
         <v>111</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123">
         <v>112</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+    <row r="124" spans="1:3">
+      <c r="A124">
         <v>112</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124">
         <v>113</v>
       </c>
       <c r="C124">
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+    <row r="125" spans="1:3">
+      <c r="A125">
         <v>113</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125">
         <v>114</v>
       </c>
       <c r="C125">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+    <row r="126" spans="1:3">
+      <c r="A126">
         <v>114</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126">
         <v>22</v>
       </c>
       <c r="C126">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+    <row r="127" spans="1:3">
+      <c r="A127">
         <v>22</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127">
         <v>115</v>
       </c>
       <c r="C127">
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+    <row r="128" spans="1:3">
+      <c r="A128">
         <v>115</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128">
         <v>116</v>
       </c>
       <c r="C128">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+    <row r="129" spans="1:3">
+      <c r="A129">
         <v>116</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129">
         <v>24</v>
       </c>
       <c r="C129">
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+    <row r="130" spans="1:3">
+      <c r="A130">
         <v>24</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130">
         <v>117</v>
       </c>
       <c r="C130">
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+    <row r="131" spans="1:3">
+      <c r="A131">
         <v>117</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131">
         <v>118</v>
       </c>
       <c r="C131">
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+    <row r="132" spans="1:3">
+      <c r="A132">
         <v>118</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132">
         <v>119</v>
       </c>
       <c r="C132">
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+    <row r="133" spans="1:3">
+      <c r="A133">
         <v>119</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133">
         <v>120</v>
       </c>
       <c r="C133">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+    <row r="134" spans="1:3">
+      <c r="A134">
         <v>120</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B134">
         <v>121</v>
       </c>
       <c r="C134">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+    <row r="135" spans="1:3">
+      <c r="A135">
         <v>121</v>
       </c>
-      <c r="B135" s="2">
+      <c r="B135">
         <v>122</v>
       </c>
       <c r="C135">
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+    <row r="136" spans="1:3">
+      <c r="A136">
         <v>122</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B136">
         <v>123</v>
       </c>
       <c r="C136">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+    <row r="137" spans="1:3">
+      <c r="A137">
         <v>123</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B137">
         <v>124</v>
       </c>
       <c r="C137">
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+    <row r="138" spans="1:3">
+      <c r="A138">
         <v>124</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B138">
         <v>125</v>
       </c>
       <c r="C138">
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+    <row r="139" spans="1:3">
+      <c r="A139">
         <v>125</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B139">
         <v>95</v>
       </c>
       <c r="C139">
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+    <row r="140" spans="1:3">
+      <c r="A140">
         <v>95</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B140">
         <v>126</v>
       </c>
       <c r="C140">
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+    <row r="141" spans="1:3">
+      <c r="A141">
         <v>126</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B141">
         <v>127</v>
       </c>
       <c r="C141">
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+    <row r="142" spans="1:3">
+      <c r="A142">
         <v>127</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B142">
         <v>128</v>
       </c>
       <c r="C142">
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+    <row r="143" spans="1:3">
+      <c r="A143">
         <v>128</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B143">
         <v>129</v>
       </c>
       <c r="C143">
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+    <row r="144" spans="1:3">
+      <c r="A144">
         <v>129</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B144">
         <v>130</v>
       </c>
       <c r="C144">
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+    <row r="145" spans="1:3">
+      <c r="A145">
         <v>130</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145">
         <v>131</v>
       </c>
       <c r="C145">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+    <row r="146" spans="1:3">
+      <c r="A146">
         <v>131</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146">
         <v>132</v>
       </c>
       <c r="C146">
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+    <row r="147" spans="1:3">
+      <c r="A147">
         <v>132</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147">
         <v>73</v>
       </c>
       <c r="C147">
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+    <row r="148" spans="1:3">
+      <c r="A148">
         <v>73</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148">
         <v>133</v>
       </c>
       <c r="C148">
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+    <row r="149" spans="1:3">
+      <c r="A149">
         <v>133</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149">
         <v>134</v>
       </c>
       <c r="C149">
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+    <row r="150" spans="1:3">
+      <c r="A150">
         <v>134</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150">
         <v>135</v>
       </c>
       <c r="C150">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+    <row r="151" spans="1:3">
+      <c r="A151">
         <v>135</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151">
         <v>136</v>
       </c>
       <c r="C151">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+    <row r="152" spans="1:3">
+      <c r="A152">
         <v>136</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152">
         <v>55</v>
       </c>
       <c r="C152">
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="8">
+    <row r="153" spans="1:3">
+      <c r="A153">
         <v>5</v>
       </c>
-      <c r="B153" s="8">
+      <c r="B153">
         <v>66</v>
       </c>
       <c r="C153">
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="8">
+    <row r="154" spans="1:3">
+      <c r="A154">
         <v>66</v>
       </c>
-      <c r="B154" s="8">
+      <c r="B154">
         <v>137</v>
       </c>
       <c r="C154">
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="8">
+    <row r="155" spans="1:3">
+      <c r="A155">
         <v>137</v>
       </c>
-      <c r="B155" s="8">
+      <c r="B155">
         <v>138</v>
       </c>
       <c r="C155">
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="8">
+    <row r="156" spans="1:3">
+      <c r="A156">
         <v>138</v>
       </c>
-      <c r="B156" s="8">
+      <c r="B156">
         <v>139</v>
       </c>
       <c r="C156">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="8">
+    <row r="157" spans="1:3">
+      <c r="A157">
         <v>139</v>
       </c>
-      <c r="B157" s="8">
+      <c r="B157">
         <v>140</v>
       </c>
       <c r="C157">
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="8">
+    <row r="158" spans="1:3">
+      <c r="A158">
         <v>140</v>
       </c>
-      <c r="B158" s="8">
+      <c r="B158">
         <v>141</v>
       </c>
       <c r="C158">
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="8">
+    <row r="159" spans="1:3">
+      <c r="A159">
         <v>141</v>
       </c>
-      <c r="B159" s="8">
+      <c r="B159">
         <v>95</v>
       </c>
       <c r="C159">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="8">
+    <row r="160" spans="1:3">
+      <c r="A160">
         <v>95</v>
       </c>
-      <c r="B160" s="8">
+      <c r="B160">
         <v>96</v>
       </c>
       <c r="C160">
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="8">
+    <row r="161" spans="1:3">
+      <c r="A161">
         <v>96</v>
       </c>
-      <c r="B161" s="8">
+      <c r="B161">
         <v>142</v>
       </c>
       <c r="C161">
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="8">
+    <row r="162" spans="1:3">
+      <c r="A162">
         <v>142</v>
       </c>
-      <c r="B162" s="8">
+      <c r="B162">
         <v>143</v>
       </c>
       <c r="C162">
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="8">
+    <row r="163" spans="1:3">
+      <c r="A163">
         <v>143</v>
       </c>
-      <c r="B163" s="8">
+      <c r="B163">
         <v>144</v>
       </c>
       <c r="C163">
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="8">
+    <row r="164" spans="1:3">
+      <c r="A164">
         <v>144</v>
       </c>
-      <c r="B164" s="8">
+      <c r="B164">
         <v>145</v>
       </c>
       <c r="C164">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="8">
+    <row r="165" spans="1:3">
+      <c r="A165">
         <v>145</v>
       </c>
-      <c r="B165" s="8">
+      <c r="B165">
         <v>146</v>
       </c>
       <c r="C165">
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="8">
+    <row r="166" spans="1:3">
+      <c r="A166">
         <v>146</v>
       </c>
-      <c r="B166" s="8">
+      <c r="B166">
         <v>147</v>
       </c>
       <c r="C166">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="8">
+    <row r="167" spans="1:3">
+      <c r="A167">
         <v>147</v>
       </c>
-      <c r="B167" s="8">
+      <c r="B167">
         <v>148</v>
       </c>
       <c r="C167">
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="8">
+    <row r="168" spans="1:3">
+      <c r="A168">
         <v>148</v>
       </c>
-      <c r="B168" s="8">
+      <c r="B168">
         <v>149</v>
       </c>
       <c r="C168">
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="8">
+    <row r="169" spans="1:3">
+      <c r="A169">
         <v>149</v>
       </c>
-      <c r="B169" s="8">
+      <c r="B169">
         <v>150</v>
       </c>
       <c r="C169">
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="8">
+    <row r="170" spans="1:3">
+      <c r="A170">
         <v>150</v>
       </c>
-      <c r="B170" s="8">
+      <c r="B170">
         <v>151</v>
       </c>
       <c r="C170">
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="8">
+    <row r="171" spans="1:3">
+      <c r="A171">
         <v>151</v>
       </c>
-      <c r="B171" s="8">
+      <c r="B171">
         <v>152</v>
       </c>
       <c r="C171">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="8">
+    <row r="172" spans="1:3">
+      <c r="A172">
         <v>152</v>
       </c>
-      <c r="B172" s="8">
+      <c r="B172">
         <v>153</v>
       </c>
       <c r="C172">
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="8">
+    <row r="173" spans="1:3">
+      <c r="A173">
         <v>153</v>
       </c>
-      <c r="B173" s="8">
+      <c r="B173">
         <v>154</v>
       </c>
       <c r="C173">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="8">
+    <row r="174" spans="1:3">
+      <c r="A174">
         <v>154</v>
       </c>
-      <c r="B174" s="8">
+      <c r="B174">
         <v>155</v>
       </c>
       <c r="C174">
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="8">
+    <row r="175" spans="1:3">
+      <c r="A175">
         <v>155</v>
       </c>
-      <c r="B175" s="8">
+      <c r="B175">
         <v>156</v>
       </c>
       <c r="C175">
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="8">
+    <row r="176" spans="1:3">
+      <c r="A176">
         <v>156</v>
       </c>
-      <c r="B176" s="8">
+      <c r="B176">
         <v>157</v>
       </c>
       <c r="C176">
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" s="8">
+    <row r="177" spans="1:3">
+      <c r="A177">
         <v>157</v>
       </c>
-      <c r="B177" s="8">
+      <c r="B177">
         <v>158</v>
       </c>
       <c r="C177">
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="8">
+    <row r="178" spans="1:3">
+      <c r="A178">
         <v>158</v>
       </c>
-      <c r="B178" s="8">
+      <c r="B178">
         <v>236</v>
       </c>
       <c r="C178">
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" s="9">
+    <row r="179" spans="1:3">
+      <c r="A179">
         <v>159</v>
       </c>
-      <c r="B179" s="9">
+      <c r="B179">
         <v>122</v>
       </c>
       <c r="C179">
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="9">
+    <row r="180" spans="1:3">
+      <c r="A180">
         <v>122</v>
       </c>
-      <c r="B180" s="9">
+      <c r="B180">
         <v>160</v>
       </c>
       <c r="C180">
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="9">
+    <row r="181" spans="1:3">
+      <c r="A181">
         <v>160</v>
       </c>
-      <c r="B181" s="9">
+      <c r="B181">
         <v>161</v>
       </c>
       <c r="C181">
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="9">
+    <row r="182" spans="1:3">
+      <c r="A182">
         <v>161</v>
       </c>
-      <c r="B182" s="9">
+      <c r="B182">
         <v>162</v>
       </c>
       <c r="C182">
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="9">
+    <row r="183" spans="1:3">
+      <c r="A183">
         <v>162</v>
       </c>
-      <c r="B183" s="9">
+      <c r="B183">
         <v>163</v>
       </c>
       <c r="C183">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="9">
+    <row r="184" spans="1:3">
+      <c r="A184">
         <v>163</v>
       </c>
-      <c r="B184" s="9">
+      <c r="B184">
         <v>164</v>
       </c>
       <c r="C184">
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="9">
+    <row r="185" spans="1:3">
+      <c r="A185">
         <v>164</v>
       </c>
-      <c r="B185" s="9">
+      <c r="B185">
         <v>44</v>
       </c>
       <c r="C185">
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="9">
+    <row r="186" spans="1:3">
+      <c r="A186">
         <v>44</v>
       </c>
-      <c r="B186" s="9">
+      <c r="B186">
         <v>165</v>
       </c>
       <c r="C186">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="9">
+    <row r="187" spans="1:3">
+      <c r="A187">
         <v>165</v>
       </c>
-      <c r="B187" s="9">
+      <c r="B187">
         <v>11</v>
       </c>
       <c r="C187">
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="9">
+    <row r="188" spans="1:3">
+      <c r="A188">
         <v>11</v>
       </c>
-      <c r="B188" s="9">
+      <c r="B188">
         <v>166</v>
       </c>
       <c r="C188">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="9">
+    <row r="189" spans="1:3">
+      <c r="A189">
         <v>166</v>
       </c>
-      <c r="B189" s="9">
+      <c r="B189">
         <v>167</v>
       </c>
       <c r="C189">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="9">
+    <row r="190" spans="1:3">
+      <c r="A190">
         <v>167</v>
       </c>
-      <c r="B190" s="9">
+      <c r="B190">
         <v>62</v>
       </c>
       <c r="C190">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="9">
+    <row r="191" spans="1:3">
+      <c r="A191">
         <v>62</v>
       </c>
-      <c r="B191" s="9">
+      <c r="B191">
         <v>168</v>
       </c>
       <c r="C191">
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="9">
+    <row r="192" spans="1:3">
+      <c r="A192">
         <v>168</v>
       </c>
-      <c r="B192" s="9">
+      <c r="B192">
         <v>89</v>
       </c>
       <c r="C192">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" s="9">
+    <row r="193" spans="1:3">
+      <c r="A193">
         <v>89</v>
       </c>
-      <c r="B193" s="9">
+      <c r="B193">
         <v>169</v>
       </c>
       <c r="C193">
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="9">
+    <row r="194" spans="1:3">
+      <c r="A194">
         <v>169</v>
       </c>
-      <c r="B194" s="9">
+      <c r="B194">
         <v>170</v>
       </c>
       <c r="C194">
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" s="9">
+    <row r="195" spans="1:3">
+      <c r="A195">
         <v>170</v>
       </c>
-      <c r="B195" s="9">
+      <c r="B195">
         <v>171</v>
       </c>
       <c r="C195">
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="9">
+    <row r="196" spans="1:3">
+      <c r="A196">
         <v>171</v>
       </c>
-      <c r="B196" s="9">
+      <c r="B196">
         <v>52</v>
       </c>
       <c r="C196">
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="9">
+    <row r="197" spans="1:3">
+      <c r="A197">
         <v>52</v>
       </c>
-      <c r="B197" s="9">
+      <c r="B197">
         <v>65</v>
       </c>
       <c r="C197">
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="9">
+    <row r="198" spans="1:3">
+      <c r="A198">
         <v>65</v>
       </c>
-      <c r="B198" s="9">
+      <c r="B198">
         <v>172</v>
       </c>
       <c r="C198">
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="9">
+    <row r="199" spans="1:3">
+      <c r="A199">
         <v>172</v>
       </c>
-      <c r="B199" s="9">
+      <c r="B199">
         <v>138</v>
       </c>
       <c r="C199">
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="9">
+    <row r="200" spans="1:3">
+      <c r="A200">
         <v>138</v>
       </c>
-      <c r="B200" s="9">
+      <c r="B200">
         <v>173</v>
       </c>
       <c r="C200">
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="9">
+    <row r="201" spans="1:3">
+      <c r="A201">
         <v>173</v>
       </c>
-      <c r="B201" s="9">
+      <c r="B201">
         <v>174</v>
       </c>
       <c r="C201">
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="9">
+    <row r="202" spans="1:3">
+      <c r="A202">
         <v>174</v>
       </c>
-      <c r="B202" s="9">
+      <c r="B202">
         <v>175</v>
       </c>
       <c r="C202">
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" s="9">
+    <row r="203" spans="1:3">
+      <c r="A203">
         <v>175</v>
       </c>
-      <c r="B203" s="9">
+      <c r="B203">
         <v>70</v>
       </c>
       <c r="C203">
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="9">
+    <row r="204" spans="1:3">
+      <c r="A204">
         <v>70</v>
       </c>
-      <c r="B204" s="9">
+      <c r="B204">
         <v>135</v>
       </c>
       <c r="C204">
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="10">
+    <row r="205" spans="1:3">
+      <c r="A205">
         <v>113</v>
       </c>
-      <c r="B205" s="10">
+      <c r="B205">
         <v>182</v>
       </c>
       <c r="C205">
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="10">
+    <row r="206" spans="1:3">
+      <c r="A206">
         <v>182</v>
       </c>
-      <c r="B206" s="10">
+      <c r="B206">
         <v>183</v>
       </c>
       <c r="C206">
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="10">
+    <row r="207" spans="1:3">
+      <c r="A207">
         <v>183</v>
       </c>
-      <c r="B207" s="10">
+      <c r="B207">
         <v>184</v>
       </c>
       <c r="C207">
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="10">
+    <row r="208" spans="1:3">
+      <c r="A208">
         <v>184</v>
       </c>
-      <c r="B208" s="10">
+      <c r="B208">
         <v>185</v>
       </c>
       <c r="C208">
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="10">
+    <row r="209" spans="1:3">
+      <c r="A209">
         <v>185</v>
       </c>
-      <c r="B209" s="10">
+      <c r="B209">
         <v>186</v>
       </c>
       <c r="C209">
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="10">
+    <row r="210" spans="1:3">
+      <c r="A210">
         <v>186</v>
       </c>
-      <c r="B210" s="10">
+      <c r="B210">
         <v>187</v>
       </c>
       <c r="C210">
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="10">
+    <row r="211" spans="1:3">
+      <c r="A211">
         <v>187</v>
       </c>
-      <c r="B211" s="10">
+      <c r="B211">
         <v>188</v>
       </c>
       <c r="C211">
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="10">
+    <row r="212" spans="1:3">
+      <c r="A212">
         <v>188</v>
       </c>
-      <c r="B212" s="10">
+      <c r="B212">
         <v>189</v>
       </c>
       <c r="C212">
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="10">
+    <row r="213" spans="1:3">
+      <c r="A213">
         <v>189</v>
       </c>
-      <c r="B213" s="10">
+      <c r="B213">
         <v>190</v>
       </c>
       <c r="C213">
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="10">
+    <row r="214" spans="1:3">
+      <c r="A214">
         <v>190</v>
       </c>
-      <c r="B214" s="10">
+      <c r="B214">
         <v>191</v>
       </c>
       <c r="C214">
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="10">
+    <row r="215" spans="1:3">
+      <c r="A215">
         <v>191</v>
       </c>
-      <c r="B215" s="10">
+      <c r="B215">
         <v>192</v>
       </c>
       <c r="C215">
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="10">
+    <row r="216" spans="1:3">
+      <c r="A216">
         <v>192</v>
       </c>
-      <c r="B216" s="10">
+      <c r="B216">
         <v>193</v>
       </c>
       <c r="C216">
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="10">
+    <row r="217" spans="1:3">
+      <c r="A217">
         <v>193</v>
       </c>
-      <c r="B217" s="10">
+      <c r="B217">
         <v>194</v>
       </c>
       <c r="C217">
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="10">
+    <row r="218" spans="1:3">
+      <c r="A218">
         <v>194</v>
       </c>
-      <c r="B218" s="10">
+      <c r="B218">
         <v>11</v>
       </c>
       <c r="C218">
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="10">
+    <row r="219" spans="1:3">
+      <c r="A219">
         <v>11</v>
       </c>
-      <c r="B219" s="10">
+      <c r="B219">
         <v>195</v>
       </c>
       <c r="C219">
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="10">
+    <row r="220" spans="1:3">
+      <c r="A220">
         <v>195</v>
       </c>
-      <c r="B220" s="10">
+      <c r="B220">
         <v>48</v>
       </c>
       <c r="C220">
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="10">
+    <row r="221" spans="1:3">
+      <c r="A221">
         <v>48</v>
       </c>
-      <c r="B221" s="10">
+      <c r="B221">
         <v>196</v>
       </c>
       <c r="C221">
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="10">
+    <row r="222" spans="1:3">
+      <c r="A222">
         <v>196</v>
       </c>
-      <c r="B222" s="10">
+      <c r="B222">
         <v>197</v>
       </c>
       <c r="C222">
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" s="10">
+    <row r="223" spans="1:3">
+      <c r="A223">
         <v>197</v>
       </c>
-      <c r="B223" s="10">
+      <c r="B223">
         <v>198</v>
       </c>
       <c r="C223">
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="10">
+    <row r="224" spans="1:3">
+      <c r="A224">
         <v>198</v>
       </c>
-      <c r="B224" s="10">
+      <c r="B224">
         <v>92</v>
       </c>
       <c r="C224">
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="10">
+    <row r="225" spans="1:3">
+      <c r="A225">
         <v>92</v>
       </c>
-      <c r="B225" s="10">
+      <c r="B225">
         <v>199</v>
       </c>
       <c r="C225">
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="10">
+    <row r="226" spans="1:3">
+      <c r="A226">
         <v>199</v>
       </c>
-      <c r="B226" s="10">
+      <c r="B226">
         <v>139</v>
       </c>
       <c r="C226">
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="10">
+    <row r="227" spans="1:3">
+      <c r="A227">
         <v>139</v>
       </c>
-      <c r="B227" s="10">
+      <c r="B227">
         <v>200</v>
       </c>
       <c r="C227">
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="10">
+    <row r="228" spans="1:3">
+      <c r="A228">
         <v>200</v>
       </c>
-      <c r="B228" s="10">
+      <c r="B228">
         <v>173</v>
       </c>
       <c r="C228">
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="10">
+    <row r="229" spans="1:3">
+      <c r="A229">
         <v>173</v>
       </c>
-      <c r="B229" s="10">
+      <c r="B229">
         <v>201</v>
       </c>
       <c r="C229">
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="10">
+    <row r="230" spans="1:3">
+      <c r="A230">
         <v>201</v>
       </c>
-      <c r="B230" s="10">
+      <c r="B230">
         <v>67</v>
       </c>
       <c r="C230">
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="10">
+    <row r="231" spans="1:3">
+      <c r="A231">
         <v>67</v>
       </c>
-      <c r="B231" s="10">
+      <c r="B231">
         <v>202</v>
       </c>
       <c r="C231">
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="10">
+    <row r="232" spans="1:3">
+      <c r="A232">
         <v>202</v>
       </c>
-      <c r="B232" s="10">
+      <c r="B232">
         <v>203</v>
       </c>
       <c r="C232">
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="10">
+    <row r="233" spans="1:3">
+      <c r="A233">
         <v>203</v>
       </c>
-      <c r="B233" s="10">
+      <c r="B233">
         <v>204</v>
       </c>
       <c r="C233">
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="10">
+    <row r="234" spans="1:3">
+      <c r="A234">
         <v>204</v>
       </c>
-      <c r="B234" s="10">
+      <c r="B234">
         <v>205</v>
       </c>
       <c r="C234">
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="10">
+    <row r="235" spans="1:3">
+      <c r="A235">
         <v>205</v>
       </c>
-      <c r="B235" s="10">
+      <c r="B235">
         <v>206</v>
       </c>
       <c r="C235">
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
+    <row r="236" spans="1:3">
+      <c r="A236">
         <v>207</v>
       </c>
-      <c r="B236" s="3">
+      <c r="B236">
         <v>89</v>
       </c>
       <c r="C236">
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="3">
+    <row r="237" spans="1:3">
+      <c r="A237">
         <v>89</v>
       </c>
-      <c r="B237" s="3">
+      <c r="B237">
         <v>7</v>
       </c>
       <c r="C237">
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="3">
+    <row r="238" spans="1:3">
+      <c r="A238">
         <v>7</v>
       </c>
-      <c r="B238" s="3">
+      <c r="B238">
         <v>64</v>
       </c>
       <c r="C238">
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="3">
+    <row r="239" spans="1:3">
+      <c r="A239">
         <v>64</v>
       </c>
-      <c r="B239" s="3">
+      <c r="B239">
         <v>208</v>
       </c>
       <c r="C239">
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="3">
+    <row r="240" spans="1:3">
+      <c r="A240">
         <v>208</v>
       </c>
-      <c r="B240" s="3">
+      <c r="B240">
         <v>199</v>
       </c>
       <c r="C240">
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="3">
+    <row r="241" spans="1:3">
+      <c r="A241">
         <v>199</v>
       </c>
-      <c r="B241" s="3">
+      <c r="B241">
         <v>209</v>
       </c>
       <c r="C241">
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="3">
+    <row r="242" spans="1:3">
+      <c r="A242">
         <v>209</v>
       </c>
-      <c r="B242" s="3">
+      <c r="B242">
         <v>210</v>
       </c>
       <c r="C242">
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243" s="3">
+    <row r="243" spans="1:3">
+      <c r="A243">
         <v>210</v>
       </c>
-      <c r="B243" s="3">
+      <c r="B243">
         <v>211</v>
       </c>
       <c r="C243">
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244" s="3">
+    <row r="244" spans="1:3">
+      <c r="A244">
         <v>211</v>
       </c>
-      <c r="B244" s="3">
+      <c r="B244">
         <v>127</v>
       </c>
       <c r="C244">
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" s="3">
+    <row r="245" spans="1:3">
+      <c r="A245">
         <v>127</v>
       </c>
-      <c r="B245" s="3">
+      <c r="B245">
         <v>212</v>
       </c>
       <c r="C245">
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" s="3">
+    <row r="246" spans="1:3">
+      <c r="A246">
         <v>212</v>
       </c>
-      <c r="B246" s="3">
+      <c r="B246">
         <v>213</v>
       </c>
       <c r="C246">
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="3">
+    <row r="247" spans="1:3">
+      <c r="A247">
         <v>213</v>
       </c>
-      <c r="B247" s="3">
+      <c r="B247">
         <v>214</v>
       </c>
       <c r="C247">
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" s="3">
+    <row r="248" spans="1:3">
+      <c r="A248">
         <v>214</v>
       </c>
-      <c r="B248" s="3">
+      <c r="B248">
         <v>215</v>
       </c>
       <c r="C248">
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" s="3">
+    <row r="249" spans="1:3">
+      <c r="A249">
         <v>215</v>
       </c>
-      <c r="B249" s="3">
+      <c r="B249">
         <v>216</v>
       </c>
       <c r="C249">
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250" s="3">
+    <row r="250" spans="1:3">
+      <c r="A250">
         <v>216</v>
       </c>
-      <c r="B250" s="3">
+      <c r="B250">
         <v>217</v>
       </c>
       <c r="C250">
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="3">
+    <row r="251" spans="1:3">
+      <c r="A251">
         <v>217</v>
       </c>
-      <c r="B251" s="3">
+      <c r="B251">
         <v>218</v>
       </c>
       <c r="C251">
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" s="3">
+    <row r="252" spans="1:3">
+      <c r="A252">
         <v>218</v>
       </c>
-      <c r="B252" s="3">
+      <c r="B252">
         <v>219</v>
       </c>
       <c r="C252">
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" s="3">
+    <row r="253" spans="1:3">
+      <c r="A253">
         <v>219</v>
       </c>
-      <c r="B253" s="3">
+      <c r="B253">
         <v>220</v>
       </c>
       <c r="C253">
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" s="3">
+    <row r="254" spans="1:3">
+      <c r="A254">
         <v>220</v>
       </c>
-      <c r="B254" s="3">
+      <c r="B254">
         <v>221</v>
       </c>
       <c r="C254">
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255" s="3">
+    <row r="255" spans="1:3">
+      <c r="A255">
         <v>221</v>
       </c>
-      <c r="B255" s="3">
+      <c r="B255">
         <v>222</v>
       </c>
       <c r="C255">
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256" s="3">
+    <row r="256" spans="1:3">
+      <c r="A256">
         <v>222</v>
       </c>
-      <c r="B256" s="3">
+      <c r="B256">
         <v>223</v>
       </c>
       <c r="C256">
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" s="3">
+    <row r="257" spans="1:3">
+      <c r="A257">
         <v>223</v>
       </c>
-      <c r="B257" s="3">
+      <c r="B257">
         <v>224</v>
       </c>
       <c r="C257">
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" s="4">
+    <row r="258" spans="1:3">
+      <c r="A258">
         <v>50</v>
       </c>
-      <c r="B258" s="4">
+      <c r="B258">
         <v>11</v>
       </c>
       <c r="C258">
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259" s="4">
+    <row r="259" spans="1:3">
+      <c r="A259">
         <v>11</v>
       </c>
-      <c r="B259" s="4">
+      <c r="B259">
         <v>191</v>
       </c>
       <c r="C259">
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" s="4">
+    <row r="260" spans="1:3">
+      <c r="A260">
         <v>191</v>
       </c>
-      <c r="B260" s="4">
+      <c r="B260">
         <v>39</v>
       </c>
       <c r="C260">
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261" s="4">
+    <row r="261" spans="1:3">
+      <c r="A261">
         <v>39</v>
       </c>
-      <c r="B261" s="4">
+      <c r="B261">
         <v>225</v>
       </c>
       <c r="C261">
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" s="4">
+    <row r="262" spans="1:3">
+      <c r="A262">
         <v>225</v>
       </c>
-      <c r="B262" s="4">
+      <c r="B262">
         <v>22</v>
       </c>
       <c r="C262">
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263" s="4">
+    <row r="263" spans="1:3">
+      <c r="A263">
         <v>22</v>
       </c>
-      <c r="B263" s="4">
+      <c r="B263">
         <v>226</v>
       </c>
       <c r="C263">
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" s="4">
+    <row r="264" spans="1:3">
+      <c r="A264">
         <v>226</v>
       </c>
-      <c r="B264" s="4">
+      <c r="B264">
         <v>227</v>
       </c>
       <c r="C264">
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265" s="4">
+    <row r="265" spans="1:3">
+      <c r="A265">
         <v>227</v>
       </c>
-      <c r="B265" s="4">
+      <c r="B265">
         <v>228</v>
       </c>
       <c r="C265">
         <v>7</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266" s="4">
+    <row r="266" spans="1:3">
+      <c r="A266">
         <v>228</v>
       </c>
-      <c r="B266" s="4">
+      <c r="B266">
         <v>229</v>
       </c>
       <c r="C266">
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267" s="4">
+    <row r="267" spans="1:3">
+      <c r="A267">
         <v>229</v>
       </c>
-      <c r="B267" s="4">
+      <c r="B267">
         <v>230</v>
       </c>
       <c r="C267">
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" s="4">
+    <row r="268" spans="1:3">
+      <c r="A268">
         <v>230</v>
       </c>
-      <c r="B268" s="4">
+      <c r="B268">
         <v>231</v>
       </c>
       <c r="C268">
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" s="4">
+    <row r="269" spans="1:3">
+      <c r="A269">
         <v>231</v>
       </c>
-      <c r="B269" s="4">
+      <c r="B269">
         <v>232</v>
       </c>
       <c r="C269">
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A270" s="4">
+    <row r="270" spans="1:3">
+      <c r="A270">
         <v>232</v>
       </c>
-      <c r="B270" s="4">
+      <c r="B270">
         <v>233</v>
       </c>
       <c r="C270">
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A271" s="4">
+    <row r="271" spans="1:3">
+      <c r="A271">
         <v>233</v>
       </c>
-      <c r="B271" s="4">
+      <c r="B271">
         <v>234</v>
       </c>
       <c r="C271">
         <v>3</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" s="4">
+    <row r="272" spans="1:3">
+      <c r="A272">
         <v>234</v>
       </c>
-      <c r="B272" s="4">
+      <c r="B272">
         <v>235</v>
       </c>
       <c r="C272">
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" s="4">
+    <row r="273" spans="1:3">
+      <c r="A273">
         <v>235</v>
       </c>
-      <c r="B273" s="4">
+      <c r="B273">
         <v>236</v>
       </c>
       <c r="C273">
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" s="4">
+    <row r="274" spans="1:3">
+      <c r="A274">
         <v>236</v>
       </c>
-      <c r="B274" s="4">
+      <c r="B274">
         <v>237</v>
       </c>
       <c r="C274">
         <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275">
+        <v>0</v>
+      </c>
+      <c r="B275">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>